<commit_message>
some change to active product
d0119
</commit_message>
<xml_diff>
--- a/prouduct_sample_active_inSite.xlsx
+++ b/prouduct_sample_active_inSite.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22668" windowHeight="4152"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22665" windowHeight="4155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>des</t>
   </si>
@@ -230,6 +230,18 @@
                                                                               مناسب استفاده در چه مکانی است؟
 مهمانی های خاص، مهمانی های شبانه، قرار عاشقانه، جلسات مهم
 </t>
+  </si>
+  <si>
+    <t>oldName</t>
+  </si>
+  <si>
+    <t>ونوم تاپ ایکستریم</t>
+  </si>
+  <si>
+    <t>کارن تاپ ایکستریم</t>
+  </si>
+  <si>
+    <t>لیدی گاگا تاپ ایکستریم</t>
   </si>
 </sst>
 </file>
@@ -551,22 +563,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.296875" customWidth="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="221.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.25" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="221.625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -574,16 +586,19 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -591,16 +606,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -608,16 +626,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -625,16 +646,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -642,16 +666,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="138" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -659,16 +686,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="138" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -679,13 +709,16 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -696,13 +729,16 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="179.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -710,16 +746,19 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="138" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -730,13 +769,16 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="165.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="171" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -747,13 +789,16 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="151.80000000000001" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -761,16 +806,19 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="151.80000000000001" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -778,12 +826,15 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>